<commit_message>
updates for Hastriter notes
</commit_message>
<xml_diff>
--- a/input/Lewis World Genera List 2 JULY 2021.xlsx
+++ b/input/Lewis World Genera List 2 JULY 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18c1f91d246f9ff5/Documents/GitHub/tpt-siphonaptera/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C658F84-25D2-483B-BCF4-C54FF823C5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCFCF1FD-45AE-4FF6-A3FD-5E1433E3B2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="395">
   <si>
     <t>AUTHOR(S)</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Li, Xie &amp; Gong</t>
-  </si>
-  <si>
-    <t>(Traub)</t>
   </si>
   <si>
     <t>Liu, Wu &amp; Wang</t>
@@ -1609,7 +1606,7 @@
   <dimension ref="A1:F259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C260" sqref="C260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -1625,13 +1622,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>363</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
@@ -1640,16 +1637,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -1660,13 +1657,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -1677,13 +1674,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C4" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -1694,13 +1691,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -1711,13 +1708,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="C6" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
@@ -1728,13 +1725,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="C7" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -1745,13 +1742,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
@@ -1762,13 +1759,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>2</v>
@@ -1779,11 +1776,11 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
@@ -1794,13 +1791,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
@@ -1811,13 +1808,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="C12" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -1828,13 +1825,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
@@ -1845,13 +1842,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>15</v>
@@ -1862,13 +1859,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>2</v>
@@ -1879,13 +1876,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>14</v>
@@ -1896,13 +1893,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
@@ -1913,13 +1910,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>14</v>
@@ -1930,11 +1927,11 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>19</v>
@@ -1945,13 +1942,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -1962,13 +1959,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>6</v>
@@ -1979,13 +1976,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>5</v>
@@ -1996,13 +1993,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>5</v>
@@ -2013,11 +2010,11 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>2</v>
@@ -2028,13 +2025,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>74</v>
-      </c>
       <c r="C25" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>25</v>
@@ -2043,18 +2040,18 @@
         <v>2015</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="C26" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>5</v>
@@ -2065,11 +2062,11 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>3</v>
@@ -2080,11 +2077,11 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>10</v>
@@ -2095,13 +2092,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="C29" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>2</v>
@@ -2112,13 +2109,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>2</v>
@@ -2129,13 +2126,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="C31" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>6</v>
@@ -2146,11 +2143,11 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>10</v>
@@ -2161,13 +2158,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>14</v>
@@ -2178,11 +2175,11 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>6</v>
@@ -2193,16 +2190,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E35" s="3">
         <v>1965</v>
@@ -2210,13 +2207,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>7</v>
@@ -2227,16 +2224,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E37" s="3">
         <v>1965</v>
@@ -2244,13 +2241,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>5</v>
@@ -2261,13 +2258,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C39" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>14</v>
@@ -2278,13 +2275,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>21</v>
@@ -2295,13 +2292,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B41" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>7</v>
@@ -2312,13 +2309,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>6</v>
@@ -2329,16 +2326,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C43" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E43" s="3">
         <v>1832</v>
@@ -2346,14 +2343,14 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E44" s="3">
         <v>1903</v>
@@ -2361,16 +2358,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="C45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="D45" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E45" s="3">
         <v>1910</v>
@@ -2378,13 +2375,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>7</v>
@@ -2395,13 +2392,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B47" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>7</v>
@@ -2412,13 +2409,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B48" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C48" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>18</v>
@@ -2429,16 +2426,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C49" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E49" s="3">
         <v>1908</v>
@@ -2446,14 +2443,14 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A50" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E50" s="3">
         <v>1922</v>
@@ -2461,13 +2458,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A51" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C51" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>14</v>
@@ -2478,13 +2475,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A52" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B52" s="12" t="s">
-        <v>110</v>
-      </c>
       <c r="C52" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>7</v>
@@ -2495,13 +2492,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A53" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>20</v>
@@ -2512,13 +2509,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B54" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C54" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>15</v>
@@ -2529,16 +2526,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B55" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C55" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E55" s="3">
         <v>1973</v>
@@ -2546,11 +2543,11 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>5</v>
@@ -2561,16 +2558,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B57" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="D57" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E57" s="3">
         <v>1973</v>
@@ -2578,13 +2575,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="C58" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>14</v>
@@ -2595,13 +2592,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A59" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B59" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>148</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>21</v>
@@ -2612,13 +2609,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A60" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B60" s="12" t="s">
-        <v>110</v>
-      </c>
       <c r="C60" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>7</v>
@@ -2629,13 +2626,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A61" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B61" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
@@ -2646,16 +2643,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A62" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B62" s="12" t="s">
-        <v>129</v>
-      </c>
       <c r="C62" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E62" s="3">
         <v>1949</v>
@@ -2663,11 +2660,11 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A63" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>6</v>
@@ -2678,16 +2675,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A64" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E64" s="3">
         <v>1930</v>
@@ -2695,13 +2692,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A65" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B65" s="12" t="s">
-        <v>101</v>
-      </c>
       <c r="C65" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>7</v>
@@ -2712,16 +2709,16 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A66" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E66" s="3">
         <v>1856</v>
@@ -2729,13 +2726,13 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B67" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C67" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>14</v>
@@ -2746,13 +2743,13 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A68" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B68" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>159</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>6</v>
@@ -2763,13 +2760,13 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A69" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B69" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C69" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>2</v>
@@ -2780,13 +2777,13 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A70" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B70" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C70" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -2797,13 +2794,13 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A71" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>6</v>
@@ -2814,13 +2811,13 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A72" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B72" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>6</v>
@@ -2832,13 +2829,13 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A73" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>6</v>
@@ -2849,16 +2846,16 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A74" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E74" s="3">
         <v>1956</v>
@@ -2866,13 +2863,13 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A75" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B75" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B75" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C75" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>17</v>
@@ -2883,13 +2880,13 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A76" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B76" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>5</v>
@@ -2900,13 +2897,13 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A77" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B77" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C77" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>13</v>
@@ -2917,13 +2914,13 @@
     </row>
     <row r="78" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A78" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B78" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B78" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="C78" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>5</v>
@@ -2935,11 +2932,11 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A79" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B79" s="12"/>
       <c r="C79" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>15</v>
@@ -2950,16 +2947,16 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E80" s="3">
         <v>1886</v>
@@ -2967,13 +2964,13 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A81" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>6</v>
@@ -2984,13 +2981,13 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A82" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>17</v>
@@ -3001,36 +2998,36 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A83" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B83" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B83" s="12" t="s">
-        <v>74</v>
-      </c>
       <c r="C83" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E83" s="7">
         <v>2012</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A84" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E84" s="3">
         <v>1940</v>
@@ -3038,13 +3035,13 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A85" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>6</v>
@@ -3055,13 +3052,13 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A86" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>6</v>
@@ -3072,11 +3069,11 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A87" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B87" s="12"/>
       <c r="C87" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>2</v>
@@ -3087,13 +3084,13 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A88" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B88" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B88" s="12" t="s">
-        <v>74</v>
-      </c>
       <c r="C88" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>8</v>
@@ -3104,13 +3101,13 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A89" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B89" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B89" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C89" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>2</v>
@@ -3121,11 +3118,11 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A90" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B90" s="12"/>
       <c r="C90" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>10</v>
@@ -3136,13 +3133,13 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A91" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>14</v>
@@ -3153,16 +3150,16 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A92" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B92" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B92" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C92" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E92" s="3">
         <v>1926</v>
@@ -3170,16 +3167,16 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A93" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E93" s="3">
         <v>1966</v>
@@ -3187,14 +3184,14 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A94" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B94" s="12"/>
       <c r="C94" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E94" s="3">
         <v>1972</v>
@@ -3202,13 +3199,13 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A95" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B95" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B95" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="C95" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>22</v>
@@ -3219,13 +3216,13 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A96" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B96" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B96" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C96" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>6</v>
@@ -3236,16 +3233,16 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A97" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B97" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B97" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C97" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E97" s="3">
         <v>1962</v>
@@ -3253,11 +3250,11 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A98" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B98" s="12"/>
       <c r="C98" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>10</v>
@@ -3268,14 +3265,14 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A99" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B99" s="12"/>
       <c r="C99" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E99" s="3">
         <v>2002</v>
@@ -3283,31 +3280,31 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A100" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B100" s="12"/>
       <c r="C100" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E100" s="3">
         <v>2013</v>
       </c>
       <c r="F100" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A101" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B101" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="C101" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>22</v>
@@ -3318,14 +3315,14 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A102" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B102" s="12"/>
       <c r="C102" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E102" s="3">
         <v>1860</v>
@@ -3333,13 +3330,13 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A103" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B103" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B103" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C103" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>10</v>
@@ -3350,11 +3347,11 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A104" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B104" s="12"/>
       <c r="C104" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>10</v>
@@ -3365,13 +3362,13 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A105" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B105" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B105" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C105" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>10</v>
@@ -3382,13 +3379,13 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A106" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B106" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B106" s="12" t="s">
-        <v>74</v>
-      </c>
       <c r="C106" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -3399,13 +3396,13 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A107" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B107" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B107" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C107" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>5</v>
@@ -3416,13 +3413,13 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A108" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>5</v>
@@ -3433,16 +3430,16 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A109" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B109" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B109" s="12" t="s">
-        <v>101</v>
-      </c>
       <c r="C109" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E109" s="3">
         <v>1880</v>
@@ -3450,13 +3447,13 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A110" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B110" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B110" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="C110" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>2</v>
@@ -3467,11 +3464,11 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A111" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B111" s="12"/>
       <c r="C111" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>6</v>
@@ -3482,13 +3479,13 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A112" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B112" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B112" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C112" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>2</v>
@@ -3499,16 +3496,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A113" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B113" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B113" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C113" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E113" s="3">
         <v>1833</v>
@@ -3516,13 +3513,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A114" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B114" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B114" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C114" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>10</v>
@@ -3533,16 +3530,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A115" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E115" s="3">
         <v>1951</v>
@@ -3550,13 +3547,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A116" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B116" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B116" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C116" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>10</v>
@@ -3567,13 +3564,13 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A117" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B117" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B117" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C117" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>5</v>
@@ -3584,11 +3581,11 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A118" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B118" s="12"/>
       <c r="C118" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>10</v>
@@ -3599,13 +3596,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A119" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>5</v>
@@ -3616,13 +3613,13 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A120" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B120" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B120" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C120" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>6</v>
@@ -3633,13 +3630,13 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A121" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>6</v>
@@ -3650,13 +3647,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A122" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B122" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>7</v>
@@ -3667,16 +3664,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A123" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B123" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="D123" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E123" s="3">
         <v>1985</v>
@@ -3684,13 +3681,13 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A124" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>7</v>
@@ -3701,13 +3698,13 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A125" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>7</v>
@@ -3718,16 +3715,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A126" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E126" s="3">
         <v>1958</v>
@@ -3735,13 +3732,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A127" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B127" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B127" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C127" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>8</v>
@@ -3752,14 +3749,14 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A128" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B128" s="12"/>
       <c r="C128" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E128" s="3">
         <v>1881</v>
@@ -3767,13 +3764,13 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A129" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B129" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B129" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C129" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>6</v>
@@ -3784,13 +3781,13 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A130" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B130" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B130" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C130" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>2</v>
@@ -3801,11 +3798,11 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A131" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B131" s="12"/>
       <c r="C131" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>10</v>
@@ -3816,13 +3813,13 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A132" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B132" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B132" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C132" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>6</v>
@@ -3833,13 +3830,13 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A133" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>5</v>
@@ -3850,16 +3847,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A134" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B134" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B134" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C134" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E134" s="3">
         <v>1980</v>
@@ -3867,13 +3864,13 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A135" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B135" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>6</v>
@@ -3884,16 +3881,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A136" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B136" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B136" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C136" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E136" s="3">
         <v>1910</v>
@@ -3901,11 +3898,11 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A137" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B137" s="12"/>
       <c r="C137" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>3</v>
@@ -3916,16 +3913,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A138" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B138" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B138" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C138" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E138" s="3">
         <v>1979</v>
@@ -3933,13 +3930,13 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A139" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B139" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B139" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C139" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>7</v>
@@ -3950,13 +3947,13 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A140" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B140" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B140" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C140" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>4</v>
@@ -3967,13 +3964,13 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A141" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B141" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>7</v>
@@ -3984,16 +3981,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A142" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B142" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B142" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C142" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E142" s="3">
         <v>1857</v>
@@ -4001,14 +3998,14 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A143" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B143" s="12"/>
       <c r="C143" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E143" s="3">
         <v>1969</v>
@@ -4016,14 +4013,14 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A144" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B144" s="12"/>
       <c r="C144" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E144" s="3">
         <v>2016</v>
@@ -4031,13 +4028,13 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A145" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B145" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B145" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C145" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>5</v>
@@ -4048,13 +4045,13 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A146" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B146" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B146" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C146" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>14</v>
@@ -4065,13 +4062,13 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A147" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B147" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>7</v>
@@ -4082,13 +4079,13 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A148" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>14</v>
@@ -4099,16 +4096,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A149" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B149" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B149" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="C149" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E149" s="3">
         <v>1993</v>
@@ -4116,11 +4113,11 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A150" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B150" s="12"/>
       <c r="C150" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>2</v>
@@ -4131,13 +4128,13 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A151" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>7</v>
@@ -4148,13 +4145,13 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A152" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>10</v>
@@ -4165,28 +4162,28 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A153" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B153" s="12"/>
       <c r="C153" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E153" s="3">
-        <v>1951</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A154" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B154" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B154" s="12" t="s">
-        <v>110</v>
-      </c>
       <c r="C154" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>14</v>
@@ -4197,13 +4194,13 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A155" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B155" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B155" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C155" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>6</v>
@@ -4214,11 +4211,11 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A156" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B156" s="12"/>
       <c r="C156" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>5</v>
@@ -4229,16 +4226,16 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A157" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B157" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B157" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C157" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E157" s="3">
         <v>1906</v>
@@ -4246,11 +4243,11 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A158" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B158" s="12"/>
       <c r="C158" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>3</v>
@@ -4261,13 +4258,13 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A159" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B159" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B159" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C159" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>15</v>
@@ -4278,13 +4275,13 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A160" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B160" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B160" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C160" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>13</v>
@@ -4295,16 +4292,16 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A161" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B161" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B161" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C161" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E161" s="3">
         <v>1926</v>
@@ -4312,13 +4309,13 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A162" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B162" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B162" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C162" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>6</v>
@@ -4329,13 +4326,13 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A163" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B163" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B163" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C163" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>6</v>
@@ -4346,16 +4343,16 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A164" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B164" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B164" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C164" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E164" s="3">
         <v>1957</v>
@@ -4363,13 +4360,13 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A165" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B165" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B165" s="12" t="s">
-        <v>74</v>
-      </c>
       <c r="C165" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>7</v>
@@ -4380,16 +4377,16 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A166" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B166" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B166" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C166" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E166" s="7">
         <v>1926</v>
@@ -4397,11 +4394,11 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A167" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B167" s="12"/>
       <c r="C167" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>3</v>
@@ -4412,13 +4409,13 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A168" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B168" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B168" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C168" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>6</v>
@@ -4429,11 +4426,11 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A169" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B169" s="12"/>
       <c r="C169" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>2</v>
@@ -4444,13 +4441,13 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A170" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B170" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>14</v>
@@ -4461,11 +4458,11 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A171" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B171" s="12"/>
       <c r="C171" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>3</v>
@@ -4476,13 +4473,13 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A172" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B172" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B172" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C172" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>14</v>
@@ -4493,13 +4490,13 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A173" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B173" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>14</v>
@@ -4510,16 +4507,16 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A174" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B174" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B174" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C174" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E174" s="3">
         <v>1909</v>
@@ -4527,13 +4524,13 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A175" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B175" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B175" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C175" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>17</v>
@@ -4544,16 +4541,16 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A176" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B176" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E176" s="3">
         <v>1937</v>
@@ -4561,16 +4558,16 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A177" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B177" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E177" s="3">
         <v>1903</v>
@@ -4578,13 +4575,13 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A178" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B178" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C178" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>14</v>
@@ -4595,11 +4592,11 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A179" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B179" s="12"/>
       <c r="C179" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>3</v>
@@ -4610,13 +4607,13 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A180" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B180" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B180" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C180" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>4</v>
@@ -4627,13 +4624,13 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A181" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B181" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>8</v>
@@ -4644,13 +4641,13 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A182" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B182" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>5</v>
@@ -4661,13 +4658,13 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A183" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B183" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>16</v>
@@ -4678,14 +4675,14 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A184" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B184" s="12"/>
       <c r="C184" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E184" s="3">
         <v>1994</v>
@@ -4693,13 +4690,13 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A185" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B185" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B185" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C185" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>6</v>
@@ -4710,13 +4707,13 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A186" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B186" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>7</v>
@@ -4727,11 +4724,11 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A187" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B187" s="12"/>
       <c r="C187" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>14</v>
@@ -4742,13 +4739,13 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A188" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B188" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B188" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C188" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>6</v>
@@ -4759,13 +4756,13 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A189" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B189" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B189" s="12" t="s">
-        <v>110</v>
-      </c>
       <c r="C189" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>6</v>
@@ -4776,13 +4773,13 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A190" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B190" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B190" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C190" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>2</v>
@@ -4793,13 +4790,13 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A191" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B191" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B191" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="C191" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>6</v>
@@ -4810,13 +4807,13 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A192" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B192" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B192" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C192" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>6</v>
@@ -4827,16 +4824,16 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A193" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B193" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B193" s="12" t="s">
-        <v>129</v>
-      </c>
       <c r="C193" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E193" s="3">
         <v>1927</v>
@@ -4844,13 +4841,13 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A194" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B194" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>6</v>
@@ -4861,34 +4858,34 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A195" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B195" s="12"/>
       <c r="C195" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E195" s="3">
         <v>2012</v>
       </c>
       <c r="F195" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A196" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B196" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B196" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C196" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E196" s="3">
         <v>2002</v>
@@ -4896,13 +4893,13 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A197" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B197" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B197" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C197" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D197" s="1" t="s">
         <v>5</v>
@@ -4913,16 +4910,16 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A198" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B198" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E198" s="3">
         <v>1758</v>
@@ -4930,13 +4927,13 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A199" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B199" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D199" s="1" t="s">
         <v>2</v>
@@ -4947,11 +4944,11 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A200" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B200" s="12"/>
       <c r="C200" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D200" s="1" t="s">
         <v>7</v>
@@ -4962,11 +4959,11 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A201" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B201" s="12"/>
       <c r="C201" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D201" s="1" t="s">
         <v>3</v>
@@ -4977,13 +4974,13 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A202" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B202" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>5</v>
@@ -4994,16 +4991,16 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A203" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B203" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B203" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C203" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E203" s="3">
         <v>1909</v>
@@ -5011,13 +5008,13 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A204" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B204" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B204" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="C204" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>13</v>
@@ -5028,13 +5025,13 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A205" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B205" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B205" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C205" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>2</v>
@@ -5045,16 +5042,16 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A206" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B206" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B206" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C206" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E206" s="3">
         <v>1926</v>
@@ -5062,13 +5059,13 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A207" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B207" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>2</v>
@@ -5079,13 +5076,13 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A208" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B208" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B208" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C208" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>9</v>
@@ -5096,13 +5093,13 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A209" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B209" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B209" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C209" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>4</v>
@@ -5113,34 +5110,34 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A210" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B210" s="12"/>
       <c r="C210" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E210" s="3">
         <v>1976</v>
       </c>
       <c r="F210" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A211" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B211" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B211" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="C211" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E211" s="3">
         <v>1968</v>
@@ -5148,13 +5145,13 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A212" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B212" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B212" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C212" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D212" s="1" t="s">
         <v>2</v>
@@ -5165,13 +5162,13 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A213" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B213" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D213" s="1" t="s">
         <v>10</v>
@@ -5182,11 +5179,11 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A214" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B214" s="12"/>
       <c r="C214" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D214" s="1" t="s">
         <v>10</v>
@@ -5197,13 +5194,13 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A215" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B215" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B215" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C215" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D215" s="1" t="s">
         <v>4</v>
@@ -5214,13 +5211,13 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A216" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B216" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B216" s="12" t="s">
-        <v>110</v>
-      </c>
       <c r="C216" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D216" s="1" t="s">
         <v>6</v>
@@ -5231,13 +5228,13 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A217" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B217" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D217" s="1" t="s">
         <v>16</v>
@@ -5248,13 +5245,13 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A218" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B218" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B218" s="12" t="s">
-        <v>74</v>
-      </c>
       <c r="C218" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D218" s="5" t="s">
         <v>13</v>
@@ -5265,13 +5262,13 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A219" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B219" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B219" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C219" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>26</v>
@@ -5282,13 +5279,13 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A220" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B220" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D220" s="1" t="s">
         <v>6</v>
@@ -5299,13 +5296,13 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A221" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B221" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>7</v>
@@ -5316,13 +5313,13 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A222" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B222" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C222" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>319</v>
       </c>
       <c r="D222" s="1" t="s">
         <v>5</v>
@@ -5333,16 +5330,16 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A223" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B223" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E223" s="3">
         <v>1893</v>
@@ -5350,13 +5347,13 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A224" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B224" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D224" s="1" t="s">
         <v>7</v>
@@ -5367,13 +5364,13 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A225" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B225" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B225" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C225" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>5</v>
@@ -5384,11 +5381,11 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A226" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B226" s="12"/>
       <c r="C226" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D226" s="1" t="s">
         <v>5</v>
@@ -5399,13 +5396,13 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A227" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B227" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D227" s="1" t="s">
         <v>10</v>
@@ -5416,11 +5413,11 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A228" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B228" s="12"/>
       <c r="C228" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D228" s="1" t="s">
         <v>3</v>
@@ -5431,13 +5428,13 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A229" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B229" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B229" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C229" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D229" s="1" t="s">
         <v>10</v>
@@ -5448,16 +5445,16 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A230" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B230" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E230" s="3">
         <v>1932</v>
@@ -5465,13 +5462,13 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A231" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B231" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D231" s="1" t="s">
         <v>6</v>
@@ -5482,13 +5479,13 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A232" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B232" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D232" s="1" t="s">
         <v>6</v>
@@ -5499,13 +5496,13 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A233" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B233" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B233" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C233" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D233" s="2" t="s">
         <v>14</v>
@@ -5516,31 +5513,31 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A234" s="12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B234" s="12"/>
       <c r="C234" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D234" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="D234" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="E234" s="3">
         <v>1986</v>
       </c>
       <c r="F234" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A235" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B235" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D235" s="1" t="s">
         <v>6</v>
@@ -5551,13 +5548,13 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A236" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B236" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="C236" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="D236" s="1" t="s">
         <v>7</v>
@@ -5568,13 +5565,13 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A237" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B237" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B237" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C237" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D237" s="2" t="s">
         <v>6</v>
@@ -5585,13 +5582,13 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A238" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B238" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B238" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="C238" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D238" s="1" t="s">
         <v>6</v>
@@ -5602,13 +5599,13 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A239" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B239" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B239" s="12" t="s">
-        <v>110</v>
-      </c>
       <c r="C239" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D239" s="1" t="s">
         <v>14</v>
@@ -5619,11 +5616,11 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A240" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B240" s="12"/>
       <c r="C240" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D240" s="1" t="s">
         <v>10</v>
@@ -5634,16 +5631,16 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A241" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B241" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B241" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C241" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E241" s="3">
         <v>1976</v>
@@ -5651,11 +5648,11 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A242" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B242" s="12"/>
       <c r="C242" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D242" s="1" t="s">
         <v>2</v>
@@ -5666,13 +5663,13 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A243" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B243" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D243" s="2" t="s">
         <v>8</v>
@@ -5683,16 +5680,16 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A244" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B244" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B244" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="C244" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E244" s="3">
         <v>2009</v>
@@ -5700,13 +5697,13 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A245" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B245" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>24</v>
@@ -5717,14 +5714,14 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A246" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B246" s="12"/>
       <c r="C246" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E246" s="3">
         <v>1758</v>
@@ -5732,13 +5729,13 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A247" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B247" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B247" s="12" t="s">
-        <v>101</v>
-      </c>
       <c r="C247" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D247" s="1" t="s">
         <v>14</v>
@@ -5749,16 +5746,16 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A248" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B248" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B248" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C248" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E248" s="3">
         <v>1980</v>
@@ -5766,31 +5763,31 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A249" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B249" s="12"/>
       <c r="C249" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E249" s="3">
         <v>2013</v>
       </c>
       <c r="F249" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A250" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B250" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D250" s="1" t="s">
         <v>7</v>
@@ -5801,14 +5798,14 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A251" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B251" s="12"/>
       <c r="C251" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E251" s="3">
         <v>1885</v>
@@ -5816,16 +5813,16 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A252" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B252" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E252" s="3">
         <v>1934</v>
@@ -5833,13 +5830,13 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A253" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B253" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D253" s="1" t="s">
         <v>10</v>
@@ -5850,11 +5847,11 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A254" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B254" s="12"/>
       <c r="C254" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D254" s="1" t="s">
         <v>23</v>
@@ -5865,14 +5862,14 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A255" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B255" s="12"/>
       <c r="C255" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E255" s="3">
         <v>1972</v>
@@ -5880,13 +5877,13 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A256" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B256" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B256" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="C256" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D256" s="1" t="s">
         <v>6</v>
@@ -5897,16 +5894,16 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A257" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B257" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E257" s="3">
         <v>1907</v>
@@ -5914,11 +5911,11 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A258" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B258" s="12"/>
       <c r="C258" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D258" s="1" t="s">
         <v>5</v>
@@ -5929,11 +5926,11 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A259" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B259" s="12"/>
       <c r="C259" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D259" s="2" t="s">
         <v>2</v>

</xml_diff>